<commit_message>
ISSUES 1, ISSUES 2, ISSUES 3  Clean up
</commit_message>
<xml_diff>
--- a/result_conflitosNetwork.xlsx
+++ b/result_conflitosNetwork.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="56">
   <si>
     <t>D DetCom</t>
   </si>
@@ -22,7 +22,7 @@
     <t>D GN</t>
   </si>
   <si>
-    <t>D Xin Liu</t>
+    <t>D LouvainC</t>
   </si>
   <si>
     <t>M DetCom</t>
@@ -31,49 +31,157 @@
     <t>M GN</t>
   </si>
   <si>
-    <t>M Xin Liu</t>
+    <t>M LouvainC</t>
   </si>
   <si>
     <t>Nmi GN</t>
   </si>
   <si>
-    <t>Nmi Xin Liu</t>
-  </si>
-  <si>
-    <t>[0.495786435786]</t>
-  </si>
-  <si>
-    <t>[0.755555555556]</t>
-  </si>
-  <si>
-    <t>[0.217391304348]</t>
-  </si>
-  <si>
-    <t>[0.764285714286]</t>
-  </si>
-  <si>
-    <t>[0.545974025974]</t>
-  </si>
-  <si>
-    <t>[0.195797720798]</t>
-  </si>
-  <si>
-    <t>[0.622108046391]</t>
-  </si>
-  <si>
-    <t>[0.153215270721]</t>
-  </si>
-  <si>
-    <t>[0.0477734345335]</t>
-  </si>
-  <si>
-    <t>[0.216371418136]</t>
-  </si>
-  <si>
-    <t>[0.349460540214]</t>
-  </si>
-  <si>
-    <t>[0.114168968326]</t>
+    <t>Nmi LouvainC</t>
+  </si>
+  <si>
+    <t>[0.740740740741]</t>
+  </si>
+  <si>
+    <t>[0.791369047619]</t>
+  </si>
+  <si>
+    <t>[0.733333333333]</t>
+  </si>
+  <si>
+    <t>[0.85]</t>
+  </si>
+  <si>
+    <t>[0.872222222222]</t>
+  </si>
+  <si>
+    <t>[0.569444444444]</t>
+  </si>
+  <si>
+    <t>[0.952380952381]</t>
+  </si>
+  <si>
+    <t>[0.766666666667]</t>
+  </si>
+  <si>
+    <t>[0.838095238095]</t>
+  </si>
+  <si>
+    <t>[0.625]</t>
+  </si>
+  <si>
+    <t>[0.826785714286]</t>
+  </si>
+  <si>
+    <t>[0.642857142857]</t>
+  </si>
+  <si>
+    <t>[0.833333333333]</t>
+  </si>
+  <si>
+    <t>[0.964285714286]</t>
+  </si>
+  <si>
+    <t>[0.6]</t>
+  </si>
+  <si>
+    <t>[0.452380952381]</t>
+  </si>
+  <si>
+    <t>[0.666666666667]</t>
+  </si>
+  <si>
+    <t>[0.8]</t>
+  </si>
+  <si>
+    <t>[0.75]</t>
+  </si>
+  <si>
+    <t>[0.888888888889]</t>
+  </si>
+  <si>
+    <t>[1.0]</t>
+  </si>
+  <si>
+    <t>[0.466666666667]</t>
+  </si>
+  <si>
+    <t>[0.571428571429]</t>
+  </si>
+  <si>
+    <t>[0.784550045914]</t>
+  </si>
+  <si>
+    <t>[0.584969008264]</t>
+  </si>
+  <si>
+    <t>[0.36015625]</t>
+  </si>
+  <si>
+    <t>[0.5624]</t>
+  </si>
+  <si>
+    <t>[0.220025510204]</t>
+  </si>
+  <si>
+    <t>[0.204456508017]</t>
+  </si>
+  <si>
+    <t>[0.713017751479]</t>
+  </si>
+  <si>
+    <t>[0.457644628099]</t>
+  </si>
+  <si>
+    <t>[0.5184375]</t>
+  </si>
+  <si>
+    <t>[0.372130102041]</t>
+  </si>
+  <si>
+    <t>[0.459775086505]</t>
+  </si>
+  <si>
+    <t>[0.501784651993]</t>
+  </si>
+  <si>
+    <t>[0.134339686288]</t>
+  </si>
+  <si>
+    <t>[0.2136]</t>
+  </si>
+  <si>
+    <t>[0.0]</t>
+  </si>
+  <si>
+    <t>[0.0795454545455]</t>
+  </si>
+  <si>
+    <t>[0.0789473684211]</t>
+  </si>
+  <si>
+    <t>[0.448979591837]</t>
+  </si>
+  <si>
+    <t>[0.33950617284]</t>
+  </si>
+  <si>
+    <t>[0.400826446281]</t>
+  </si>
+  <si>
+    <t>[0.333333333333]</t>
+  </si>
+  <si>
+    <t>[0.319444444444]</t>
+  </si>
+  <si>
+    <t>[0.47520661157]</t>
+  </si>
+  <si>
+    <t>[0.205075445816]</t>
+  </si>
+  <si>
+    <t>[0.402777777778]</t>
   </si>
 </sst>
 </file>
@@ -431,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,25 +579,25 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D2">
-        <v>0.451264795692582</v>
+        <v>0.144280225893813</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G2">
-        <v>0.151066947024101</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.745614727162907</v>
+        <v>8.32667268468867e-07</v>
       </c>
       <c r="I2">
-        <v>0.596090269879963</v>
+        <v>8.32667268468867e-07</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -500,25 +608,25 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D3">
-        <v>0.451264795692582</v>
+        <v>0.144280225893813</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G3">
-        <v>0.151066947024101</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.668709669649913</v>
+        <v>5.55111512312578e-07</v>
       </c>
       <c r="I3">
-        <v>0.455892055779727</v>
+        <v>5.55111512312578e-07</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -529,25 +637,25 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D4">
-        <v>0.451264795692582</v>
+        <v>0.144280225893813</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G4">
-        <v>0.151066947024101</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0.873842785870213</v>
+        <v>1.11022302462516e-06</v>
       </c>
       <c r="I4">
-        <v>0.534721137500066</v>
+        <v>1.11022302462516e-06</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -558,25 +666,25 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>0.451264795692582</v>
+        <v>0.144280225893813</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G5">
-        <v>0.151066947024101</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.606318125020951</v>
+        <v>1.11022302462516e-06</v>
       </c>
       <c r="I5">
-        <v>0.375161857590022</v>
+        <v>1.11022302462516e-06</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -587,25 +695,808 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-5.55111512312578e-07</v>
+      </c>
+      <c r="I6">
+        <v>-5.55111512312578e-07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>0.451264795692582</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>5.55111512312578e-07</v>
+      </c>
+      <c r="I7">
+        <v>5.55111512312578e-07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>-4.9960036108132e-06</v>
+      </c>
+      <c r="I9">
+        <v>-4.9960036108132e-06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1.11022302462516e-06</v>
+      </c>
+      <c r="I10">
+        <v>1.11022302462516e-06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>-2.22044604925031e-06</v>
+      </c>
+      <c r="I11">
+        <v>-2.22044604925031e-06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>-2.77555756156289e-06</v>
+      </c>
+      <c r="I12">
+        <v>-2.77555756156289e-06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="G6">
-        <v>0.151066947024101</v>
-      </c>
-      <c r="H6">
-        <v>0.610681422567757</v>
-      </c>
-      <c r="I6">
-        <v>0.300377698329395</v>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>-1.66533453693773e-06</v>
+      </c>
+      <c r="I13">
+        <v>-1.66533453693773e-06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>-5.55111512312578e-07</v>
+      </c>
+      <c r="I14">
+        <v>-5.55111512312578e-07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1.11022302462516e-06</v>
+      </c>
+      <c r="I15">
+        <v>1.11022302462516e-06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>-1.11022302462516e-06</v>
+      </c>
+      <c r="I17">
+        <v>-1.11022302462516e-06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>4.44089209850063e-06</v>
+      </c>
+      <c r="I20">
+        <v>4.44089209850063e-06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>3.33066907387547e-06</v>
+      </c>
+      <c r="I21">
+        <v>3.33066907387547e-06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>3.33066907387547e-06</v>
+      </c>
+      <c r="I22">
+        <v>3.33066907387547e-06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>3.33066907387547e-06</v>
+      </c>
+      <c r="I24">
+        <v>3.33066907387547e-06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>2.22044604925031e-06</v>
+      </c>
+      <c r="I25">
+        <v>2.22044604925031e-06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>5.55111512312578e-07</v>
+      </c>
+      <c r="I26">
+        <v>5.55111512312578e-07</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33">
+        <v>0.144280225893813</v>
+      </c>
+      <c r="E33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>